<commit_message>
gpx_json.pl added initial version
</commit_message>
<xml_diff>
--- a/gps_documentation.xlsx
+++ b/gps_documentation.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GPX!$A$1:$H$9</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GPX!$A$1:$H$11</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="56">
   <si>
     <t>Program</t>
   </si>
@@ -43,12 +43,6 @@
   </si>
   <si>
     <t>&lt;ele&gt;</t>
-  </si>
-  <si>
-    <t>optionally remove</t>
-  </si>
-  <si>
-    <t>g.pl</t>
   </si>
   <si>
     <t>gpx.pl</t>
@@ -219,32 +213,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">joins two or more GPX files together  
-optionally removes &lt;time&gt; (date-time) and &lt;ele&gt; (elevation) tags
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Should we remove duplicate wayponts withsame name and within 10m of each other?</t>
-    </r>
-  </si>
-  <si>
-    <t>reads a GPX track file (-i) and one or more Glossary file(s) (-g). 
-It works out which places have been 'passed through' and outputs one or both of 
-    a  (-o) a JSON format file and 
-    a (-x) GPX format file. 
-The GPX format file contains the original waypoints from the input GPX file  plus additional waypoints corresponding to each of the points 'passed though'. 
-The JSON format file contains both the original track (as a "LineString" Feature), and the original waypoints (plus optionally if glossary(s) specified) each point passed through (as a series of "Point" Features). 
-Track segments in the original GPX file are respected.</t>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">reads a GPX file and removes 'stationary' points. 
 the GPX file contains one or more segments each containing a track it implements two algorithms to clean up the track -  A(B)C, and Clusterng
 outputs both a GPX and CSV file. 
@@ -260,6 +228,95 @@
         <scheme val="minor"/>
       </rPr>
       <t>The GPX file only contains a single segment.</t>
+    </r>
+  </si>
+  <si>
+    <t>optionally remove (-e)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">reads a GPX track file (-i) and one or more Glossary file(s) (-g). 
+It works out which places have been 'passed through' and outputs one or both of 
+    -o  a JSON format file and 
+    -x  GPX format file. 
+The GPX format file contains the original waypoints from the input GPX file  plus additional waypoints corresponding to each of the points 'passed though'. 
+The JSON format file contains both the original track (as a "LineString" Feature), and the original waypoints (plus optionally if glossary(s) specified) each point passed through (as a series of "Point" Features). 
+Track segments in the original GPX file are respected.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Perhaps split into two programmes - one to add places the other to outut a JSON file from GPX input</t>
+    </r>
+  </si>
+  <si>
+    <t>gpx_place.pl</t>
+  </si>
+  <si>
+    <t>gpx_json.pl</t>
+  </si>
+  <si>
+    <t>preserves all original ones and optionally adds new from glossary corresponding to places passed through</t>
+  </si>
+  <si>
+    <t>g.pl
+See gpx_place.pl and gpx_json.pl</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">joins two or more GPX files together  
+   -t removes &lt;time&gt; (date-time) tags and 
+   -e removes &lt;ele&gt; (elevation) tags
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Should we remove duplicate wayponts with same name and within 10m of each other?</t>
+    </r>
+  </si>
+  <si>
+    <t>optionally remove (-t)</t>
+  </si>
+  <si>
+    <t>reads a GPX track file, and one or more Glossary file(s). 
+It works out which places have been 'passed through' and adds them as waypoints
+    -i  input GPX file 
+    -g  one or more glossary files, and 
+    -o  output GPX file. 
+The output GPX file contains the original waypoints from the input GPX file  plus additional waypoints corresponding to each of the points 'passed though'. 
+Track segments in the original GPX file are respected.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">reads a GPX track file (-i) and outputs (-o) a JSON format file 
+    -i input GPX file
+    -o  output JSON format file. 
+The input GPX format file may contain multiple segments and waypoints.
+The output JSON format file contains both the original track segments (as a series of "LineString" Feature), and the  waypoints (as a series of "Point" Features). 
+UNDER DEVELOPMENT 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Perhaps split into two programmes - one to add places the other to outut a JSON file from GPX input</t>
     </r>
   </si>
 </sst>
@@ -325,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -350,6 +407,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -656,10 +716,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,7 +755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -704,51 +764,51 @@
         <v>4</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="180" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="150" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="1" t="s">
+    <row r="5" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>44</v>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>4</v>
@@ -758,116 +818,140 @@
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B6" s="2"/>
+      <c r="C6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="4" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="1" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="4" t="s">
+      <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="1" t="s">
-        <v>18</v>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="9" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>46</v>
+      <c r="C9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="C10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+      <c r="H10" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="H11" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
@@ -912,20 +996,20 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="1"/>
+      <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
@@ -937,10 +1021,10 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
+      <c r="A19" s="5"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -948,6 +1032,26 @@
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
     </row>
   </sheetData>
   <printOptions gridLines="1"/>
@@ -975,27 +1079,27 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="H1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>32</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -1011,49 +1115,49 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="I4" s="2"/>
     </row>
@@ -1070,42 +1174,42 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>

</xml_diff>